<commit_message>
Added databars and iconset examples
</commit_message>
<xml_diff>
--- a/EPPlus.WebSampleMvc.NetCore/data/CfExport1.xlsx
+++ b/EPPlus.WebSampleMvc.NetCore/data/CfExport1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OssianEdström\Documents\Epplus_Repos\WebSamplenewnew\EPPlus.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OssianEdström\Documents\Epplus_Repos\WebSamplesClean\EPPlus.WebSamples\EPPlus.WebSampleMvc.NetCore\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48579244-F79F-450B-B2D8-14309CD4A97E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C28BFEA4-988B-4BFC-8668-410251756AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{4CABED9D-152D-43BF-B8F7-E002A4794690}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="131">
   <si>
     <t>City</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Data Bars</t>
   </si>
   <si>
-    <t>Item</t>
-  </si>
-  <si>
     <t>June</t>
   </si>
   <si>
@@ -107,42 +104,6 @@
     <t>Difference</t>
   </si>
   <si>
-    <t>Cable TV</t>
-  </si>
-  <si>
-    <t>Car Insurance</t>
-  </si>
-  <si>
-    <t>Car Payment</t>
-  </si>
-  <si>
-    <t>Cell Phone</t>
-  </si>
-  <si>
-    <t>Electricity</t>
-  </si>
-  <si>
-    <t>Gasoline</t>
-  </si>
-  <si>
-    <t>Gym Membership</t>
-  </si>
-  <si>
-    <t>Hairdresser's</t>
-  </si>
-  <si>
-    <t>Hourse Rent</t>
-  </si>
-  <si>
-    <t>Internet</t>
-  </si>
-  <si>
-    <t>Pet Care</t>
-  </si>
-  <si>
-    <t>Student Loan</t>
-  </si>
-  <si>
     <t>Expression</t>
   </si>
   <si>
@@ -384,6 +345,90 @@
   </si>
   <si>
     <t xml:space="preserve">Year of purchase </t>
+  </si>
+  <si>
+    <t>Iconsets</t>
+  </si>
+  <si>
+    <t>Games</t>
+  </si>
+  <si>
+    <t>BG3</t>
+  </si>
+  <si>
+    <t>Sims 4</t>
+  </si>
+  <si>
+    <t>Hours 2022</t>
+  </si>
+  <si>
+    <t>Hours 2023</t>
+  </si>
+  <si>
+    <t>Super hot</t>
+  </si>
+  <si>
+    <t>Slay the spire</t>
+  </si>
+  <si>
+    <t>ME: Legendary edition</t>
+  </si>
+  <si>
+    <t>Don't Starve</t>
+  </si>
+  <si>
+    <t>Elden Ring</t>
+  </si>
+  <si>
+    <t>Minecraft</t>
+  </si>
+  <si>
+    <t>Civ 5</t>
+  </si>
+  <si>
+    <t>Duck Game</t>
+  </si>
+  <si>
+    <t>DOOM: Eternal</t>
+  </si>
+  <si>
+    <t>SmartTv</t>
+  </si>
+  <si>
+    <t>MC Insurance</t>
+  </si>
+  <si>
+    <t>MC Payment</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>Energy bill</t>
+  </si>
+  <si>
+    <t>MC fuel</t>
+  </si>
+  <si>
+    <t>Fittness membership</t>
+  </si>
+  <si>
+    <t>Haircut</t>
+  </si>
+  <si>
+    <t>House loan</t>
+  </si>
+  <si>
+    <t>Broadband</t>
+  </si>
+  <si>
+    <t>Dog food</t>
+  </si>
+  <si>
+    <t>Loan Payment</t>
+  </si>
+  <si>
+    <t>Monthly item</t>
   </si>
 </sst>
 </file>
@@ -543,7 +588,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="36">
+  <dxfs count="37">
     <dxf>
       <font>
         <b/>
@@ -720,6 +765,9 @@
           <bgColor rgb="FFD9523B"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -945,8 +993,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFED9D9B"/>
       <color rgb="FFD65656"/>
-      <color rgb="FFED9D9B"/>
       <color rgb="FFEC4A4A"/>
       <color rgb="FFE4A4A4"/>
       <color rgb="FFE44743"/>
@@ -984,14 +1032,29 @@
 </table>
 </file>
 
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{9C9A905C-2D09-48CB-BBDC-5D0CB140587F}" name="tblIconSet" displayName="tblIconSet" ref="F67:I79" totalsRowShown="0">
+  <autoFilter ref="F67:I79" xr:uid="{9C9A905C-2D09-48CB-BBDC-5D0CB140587F}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{44F1E7C2-4EEA-412C-A9B7-7AACDC04F0CC}" name="Games"/>
+    <tableColumn id="2" xr3:uid="{AA6C4468-045B-4A48-990B-D237A28402ED}" name="Hours 2022"/>
+    <tableColumn id="3" xr3:uid="{CE935084-99ED-4A4B-AAF1-264CFB961B91}" name="Hours 2023"/>
+    <tableColumn id="4" xr3:uid="{36EEE1EE-FBB6-40AE-8DCE-9E3F770956A5}" name="Difference" dataDxfId="18">
+      <calculatedColumnFormula>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C5BE3727-A729-4BD2-9382-9268C6965C42}" name="tblDataBars" displayName="tblDataBars" ref="A67:D79" totalsRowShown="0">
   <autoFilter ref="A67:D79" xr:uid="{C5BE3727-A729-4BD2-9382-9268C6965C42}"/>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{D00BC406-9FEF-482C-AC80-FA77E1F21BF2}" name="Item"/>
-    <tableColumn id="2" xr3:uid="{76E431B4-F288-434D-A793-CC01CCFF26A4}" name="June" dataDxfId="35"/>
-    <tableColumn id="3" xr3:uid="{0ED06A74-07A2-4C7D-A58D-3D118E19CF80}" name="July" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{8E522953-19FF-42A1-92AF-465D3E964839}" name="Difference" dataDxfId="33">
+    <tableColumn id="1" xr3:uid="{D00BC406-9FEF-482C-AC80-FA77E1F21BF2}" name="Monthly item"/>
+    <tableColumn id="2" xr3:uid="{76E431B4-F288-434D-A793-CC01CCFF26A4}" name="June" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{0ED06A74-07A2-4C7D-A58D-3D118E19CF80}" name="July" dataDxfId="35"/>
+    <tableColumn id="4" xr3:uid="{8E522953-19FF-42A1-92AF-465D3E964839}" name="Difference" dataDxfId="34">
       <calculatedColumnFormula>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -1011,7 +1074,7 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B53755AF-B624-4294-9552-77EFB99FBAAF}" name="averageTbl" displayName="averageTbl" ref="D28:E37" totalsRowShown="0" headerRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{B53755AF-B624-4294-9552-77EFB99FBAAF}" name="averageTbl" displayName="averageTbl" ref="D28:E37" totalsRowShown="0" headerRowDxfId="33">
   <autoFilter ref="D28:E37" xr:uid="{B53755AF-B624-4294-9552-77EFB99FBAAF}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{96E735DE-A1C1-410A-BDDA-8BBC005E9646}" name="Locations"/>
@@ -1026,16 +1089,16 @@
   <autoFilter ref="A17:D24" xr:uid="{1667A648-8A15-4FC0-8C04-51C30B353BA9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{779307DB-7878-414C-93FD-F2200869FB37}" name="Wireless earbuds"/>
-    <tableColumn id="2" xr3:uid="{5B36E36F-5CF5-43EF-AFD0-2BB355AFB152}" name="Price " dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{5B36E36F-5CF5-43EF-AFD0-2BB355AFB152}" name="Price " dataDxfId="32"/>
     <tableColumn id="3" xr3:uid="{52897D8D-5C6E-474A-BD7D-7347CFD12E88}" name="Color Options "/>
-    <tableColumn id="4" xr3:uid="{4C8F154B-A419-4C4B-A46E-FEA25C6A3060}" name="Expected update " dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{4C8F154B-A419-4C4B-A46E-FEA25C6A3060}" name="Expected update " dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{1858E26A-8F53-4623-AFAA-013D115D53B9}" name="blanksTbl" displayName="blanksTbl" ref="F17:I24" totalsRowShown="0" headerRowDxfId="29">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{1858E26A-8F53-4623-AFAA-013D115D53B9}" name="blanksTbl" displayName="blanksTbl" ref="F17:I24" totalsRowShown="0" headerRowDxfId="30">
   <autoFilter ref="F17:I24" xr:uid="{1858E26A-8F53-4623-AFAA-013D115D53B9}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{9E753DAE-994A-47D2-8211-3E40EA31EB9D}" name="Employee"/>
@@ -1048,29 +1111,29 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FCAA250E-855B-41AE-97AB-D7C285C7DEB9}" name="top10Tbl" displayName="top10Tbl" ref="A28:B40" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{FCAA250E-855B-41AE-97AB-D7C285C7DEB9}" name="top10Tbl" displayName="top10Tbl" ref="A28:B40" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A28:B40" xr:uid="{FCAA250E-855B-41AE-97AB-D7C285C7DEB9}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{55A47A86-D756-4F4B-91DC-2A60F981D702}" name="Videogames" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{D3F1A5A9-FC88-45C6-B782-2857884DF250}" name="Metacritic score" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{55A47A86-D756-4F4B-91DC-2A60F981D702}" name="Videogames" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{D3F1A5A9-FC88-45C6-B782-2857884DF250}" name="Metacritic score" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{13749D1F-93BD-42C0-9AF0-E7A4E4D6ECFB}" name="uniqueDuplicatesTbl" displayName="uniqueDuplicatesTbl" ref="A44:B52" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22" totalsRowBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{13749D1F-93BD-42C0-9AF0-E7A4E4D6ECFB}" name="uniqueDuplicatesTbl" displayName="uniqueDuplicatesTbl" ref="A44:B52" totalsRowShown="0" headerRowDxfId="26" dataDxfId="24" headerRowBorderDxfId="25" tableBorderDxfId="23" totalsRowBorderDxfId="22">
   <autoFilter ref="A44:B52" xr:uid="{13749D1F-93BD-42C0-9AF0-E7A4E4D6ECFB}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{2F1A9744-59D9-49DA-9333-092C9F83B785}" name="HighScores " dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B112A37C-5FF1-4DA7-A0FD-F991E834872E}" name="Name" dataDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{2F1A9744-59D9-49DA-9333-092C9F83B785}" name="HighScores " dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B112A37C-5FF1-4DA7-A0FD-F991E834872E}" name="Name" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9C9B8040-38C8-4DAC-98DE-2ED698608E28}" name="errorsTbl" displayName="errorsTbl" ref="K17:L23" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9C9B8040-38C8-4DAC-98DE-2ED698608E28}" name="errorsTbl" displayName="errorsTbl" ref="K17:L23" totalsRowShown="0" headerRowDxfId="19">
   <autoFilter ref="K17:L23" xr:uid="{9C9B8040-38C8-4DAC-98DE-2ED698608E28}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{CD4489A5-710A-4FB8-B9F0-82ABBF6E2795}" name="Animals"/>
@@ -1399,8 +1462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE2BD51E-2CE5-4044-B083-7E3E2BAED1E8}">
   <dimension ref="A1:L79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D63" sqref="D63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1680,72 +1743,72 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="13" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="D17" s="14" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
       <c r="L17" s="13" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B18" s="19">
         <v>239</v>
       </c>
       <c r="C18" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D18" s="4">
         <f ca="1" xml:space="preserve"> TODAY() - 1</f>
-        <v>45377</v>
+        <v>45431</v>
       </c>
       <c r="F18" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="G18" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>73</v>
       </c>
       <c r="K18" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
       <c r="L18">
         <f>5000+35</f>
@@ -1754,26 +1817,26 @@
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B19" s="19">
         <v>269</v>
       </c>
       <c r="C19" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D19" s="4">
         <f ca="1">TODAY()</f>
-        <v>45378</v>
+        <v>45432</v>
       </c>
       <c r="F19" t="s">
-        <v>79</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="K19" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
       <c r="L19" t="e">
         <f>"5000T"+10</f>
@@ -1782,29 +1845,29 @@
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B20" s="19">
         <v>300</v>
       </c>
       <c r="C20" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D20" s="4">
         <f ca="1">TODAY()+1</f>
-        <v>45379</v>
+        <v>45433</v>
       </c>
       <c r="F20" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="G20" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="I20" t="s">
-        <v>87</v>
+        <v>74</v>
       </c>
       <c r="K20" t="s">
-        <v>103</v>
+        <v>90</v>
       </c>
       <c r="L20">
         <f>30+7</f>
@@ -1813,26 +1876,26 @@
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B21" s="19">
         <v>500</v>
       </c>
       <c r="C21" t="s">
-        <v>58</v>
+        <v>45</v>
       </c>
       <c r="D21" s="4">
         <f ca="1">TODAY() + 7</f>
-        <v>45385</v>
+        <v>45439</v>
       </c>
       <c r="F21" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="I21" t="s">
-        <v>96</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
-        <v>104</v>
+        <v>91</v>
       </c>
       <c r="L21" t="e">
         <f>MEDIAN(H56,Horse)</f>
@@ -1841,32 +1904,32 @@
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B22" s="19">
         <v>500000</v>
       </c>
       <c r="C22" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D22" s="4">
         <f ca="1">TODAY() + 8</f>
-        <v>45386</v>
+        <v>45440</v>
       </c>
       <c r="F22" t="s">
-        <v>82</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="H22" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" t="s">
         <v>92</v>
-      </c>
-      <c r="I22" t="s">
-        <v>88</v>
-      </c>
-      <c r="K22" t="s">
-        <v>105</v>
       </c>
       <c r="L22" t="e">
         <v>#REF!</v>
@@ -1874,29 +1937,29 @@
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="B23" s="19">
         <v>289</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>47</v>
       </c>
       <c r="D23" s="4">
         <f ca="1">TODAY() + 9</f>
-        <v>45387</v>
+        <v>45441</v>
       </c>
       <c r="F23" t="s">
-        <v>83</v>
+        <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="H23" t="s">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="K23" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="L23">
         <f>55+7</f>
@@ -1905,53 +1968,53 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="B24" s="19">
         <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="D24" s="4">
         <f ca="1">TODAY() + 10</f>
-        <v>45388</v>
+        <v>45442</v>
       </c>
       <c r="F24" t="s">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="I24" t="s">
-        <v>98</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="12" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="B29" s="10">
         <v>78</v>
@@ -1965,7 +2028,7 @@
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="12" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B30" s="11">
         <v>32</v>
@@ -1979,7 +2042,7 @@
     </row>
     <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="12" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B31" s="10">
         <v>46</v>
@@ -1993,7 +2056,7 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="12" t="s">
-        <v>64</v>
+        <v>51</v>
       </c>
       <c r="B32" s="11">
         <v>96</v>
@@ -2007,7 +2070,7 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="12" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="B33" s="10">
         <v>91</v>
@@ -2021,7 +2084,7 @@
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="12" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="B34" s="11">
         <v>92</v>
@@ -2035,7 +2098,7 @@
     </row>
     <row r="35" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B35" s="10">
         <v>79</v>
@@ -2049,7 +2112,7 @@
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="B36" s="11">
         <v>78</v>
@@ -2063,7 +2126,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="B37" s="10">
         <v>45</v>
@@ -2077,7 +2140,7 @@
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
-        <v>73</v>
+        <v>60</v>
       </c>
       <c r="B38" s="11">
         <v>97</v>
@@ -2085,7 +2148,7 @@
     </row>
     <row r="39" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="12" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B39" s="10">
         <v>84</v>
@@ -2093,7 +2156,7 @@
     </row>
     <row r="40" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="12" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="B40" s="11">
         <v>82</v>
@@ -2101,24 +2164,24 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="18" t="s">
-        <v>113</v>
+        <v>100</v>
       </c>
       <c r="B44" s="18" t="s">
-        <v>112</v>
+        <v>99</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
       <c r="E44" s="14" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2126,7 +2189,7 @@
         <v>667</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D45">
         <v>1999</v>
@@ -2140,7 +2203,7 @@
         <v>665</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D46">
         <v>2000</v>
@@ -2154,13 +2217,13 @@
         <v>420</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D47">
         <v>2001</v>
       </c>
       <c r="E47" s="8" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2168,7 +2231,7 @@
         <v>420</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D48">
         <v>2002</v>
@@ -2182,13 +2245,13 @@
         <v>355</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="D49">
         <v>2003</v>
       </c>
       <c r="E49" s="8" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2196,7 +2259,7 @@
         <v>236</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D50">
         <v>2004</v>
@@ -2210,13 +2273,13 @@
         <v>230</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D51">
         <v>2005</v>
       </c>
       <c r="E51" s="8" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -2224,228 +2287,413 @@
         <v>125</v>
       </c>
       <c r="B52" s="9" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F65" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" t="s">
         <v>19</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>20</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
         <v>21</v>
       </c>
-      <c r="D67" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
+        <v>104</v>
+      </c>
+      <c r="G67" t="s">
+        <v>107</v>
+      </c>
+      <c r="H67" t="s">
+        <v>108</v>
+      </c>
+      <c r="I67" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>23</v>
+        <v>118</v>
       </c>
       <c r="B68" s="2">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C68" s="2">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D68" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="F68" t="s">
+        <v>105</v>
+      </c>
+      <c r="G68">
+        <v>10</v>
+      </c>
+      <c r="H68">
+        <v>300</v>
+      </c>
+      <c r="I68" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>24</v>
+        <v>120</v>
       </c>
       <c r="B69" s="2">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C69" s="2">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="D69" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0.52631578947368418</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.30769230769230771</v>
+      </c>
+      <c r="F69" t="s">
+        <v>106</v>
+      </c>
+      <c r="G69">
+        <v>10</v>
+      </c>
+      <c r="H69">
+        <v>80</v>
+      </c>
+      <c r="I69" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>25</v>
+        <v>119</v>
       </c>
       <c r="B70" s="2">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C70" s="2">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D70" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>3.1578947368421054E-2</v>
+      </c>
+      <c r="F70" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70">
+        <v>2</v>
+      </c>
+      <c r="H70">
+        <v>6</v>
+      </c>
+      <c r="I70" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="B71" s="2">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C71" s="2">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D71" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-5.5555555555555552E-2</v>
+      </c>
+      <c r="F71" t="s">
+        <v>110</v>
+      </c>
+      <c r="G71">
+        <v>10</v>
+      </c>
+      <c r="H71">
+        <v>20</v>
+      </c>
+      <c r="I71" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>27</v>
+        <v>122</v>
       </c>
       <c r="B72" s="2">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C72" s="2">
-        <v>120</v>
+        <v>124</v>
       </c>
       <c r="D72" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>4.3478260869565216E-2</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+        <v>9.7345132743362831E-2</v>
+      </c>
+      <c r="F72" t="s">
+        <v>111</v>
+      </c>
+      <c r="G72">
+        <v>30</v>
+      </c>
+      <c r="H72">
+        <v>200</v>
+      </c>
+      <c r="I72" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>5.666666666666667</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>28</v>
+        <v>123</v>
       </c>
       <c r="B73" s="2">
-        <v>105</v>
+        <v>117</v>
       </c>
       <c r="C73" s="2">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="D73" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0.25714285714285712</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.14529914529914531</v>
+      </c>
+      <c r="F73" t="s">
+        <v>112</v>
+      </c>
+      <c r="G73">
+        <v>10</v>
+      </c>
+      <c r="H73">
+        <v>20</v>
+      </c>
+      <c r="I73" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>29</v>
+        <v>124</v>
       </c>
       <c r="B74" s="2">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C74" s="2">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D74" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.41666666666666669</v>
+      </c>
+      <c r="F74" t="s">
+        <v>113</v>
+      </c>
+      <c r="G74">
+        <v>150</v>
+      </c>
+      <c r="H74">
+        <v>20</v>
+      </c>
+      <c r="I74" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>-0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>30</v>
+        <v>125</v>
       </c>
       <c r="B75" s="2">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C75" s="2">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D75" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>-0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.18181818181818182</v>
+      </c>
+      <c r="F75" t="s">
+        <v>114</v>
+      </c>
+      <c r="G75">
+        <v>2</v>
+      </c>
+      <c r="H75">
+        <v>150</v>
+      </c>
+      <c r="I75" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>31</v>
+        <v>126</v>
       </c>
       <c r="B76" s="2">
-        <v>200</v>
+        <v>167</v>
       </c>
       <c r="C76" s="2">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D76" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>-0.05</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.15568862275449102</v>
+      </c>
+      <c r="F76" t="s">
+        <v>115</v>
+      </c>
+      <c r="G76">
+        <v>100</v>
+      </c>
+      <c r="H76">
+        <v>5</v>
+      </c>
+      <c r="I76" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>-0.95</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>32</v>
+        <v>127</v>
       </c>
       <c r="B77" s="2">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C77" s="2">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D77" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>-3.3333333333333333E-2</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.17391304347826086</v>
+      </c>
+      <c r="F77" t="s">
+        <v>54</v>
+      </c>
+      <c r="G77">
+        <v>20</v>
+      </c>
+      <c r="H77">
+        <v>123</v>
+      </c>
+      <c r="I77" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>5.15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>33</v>
+        <v>128</v>
       </c>
       <c r="B78" s="2">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C78" s="2">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D78" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+        <v>-0.1875</v>
+      </c>
+      <c r="F78" t="s">
+        <v>117</v>
+      </c>
+      <c r="G78">
+        <v>90</v>
+      </c>
+      <c r="H78">
+        <v>2</v>
+      </c>
+      <c r="I78" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>-0.97777777777777775</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>34</v>
+        <v>129</v>
       </c>
       <c r="B79" s="2">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="C79" s="2">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="D79" s="3">
         <f>(tblDataBars[[#This Row],[July]]-tblDataBars[[#This Row],[June]])/tblDataBars[[#This Row],[June]]</f>
-        <v>0.05</v>
+        <v>-0.17499999999999999</v>
+      </c>
+      <c r="F79" t="s">
+        <v>116</v>
+      </c>
+      <c r="G79">
+        <v>5</v>
+      </c>
+      <c r="H79">
+        <v>6</v>
+      </c>
+      <c r="I79" s="3">
+        <f>tblIconSet[[#This Row],[Hours 2023]]/tblIconSet[[#This Row],[Hours 2022]]-1</f>
+        <v>0.19999999999999996</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="A45:A52">
-    <cfRule type="duplicateValues" dxfId="17" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18:B24">
-    <cfRule type="cellIs" dxfId="16" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="30" operator="between">
       <formula>250</formula>
       <formula>300</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B29:B40">
-    <cfRule type="top10" dxfId="15" priority="1" rank="10"/>
+    <cfRule type="top10" dxfId="15" priority="6" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45:B52">
-    <cfRule type="uniqueValues" dxfId="14" priority="13"/>
-    <cfRule type="duplicateValues" dxfId="13" priority="14"/>
+    <cfRule type="uniqueValues" dxfId="14" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="19"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B68:B79">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="formula" val="30-5"/>
+        <cfvo type="formula" val="120-5"/>
+        <color rgb="FF638EC6"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{24D561F3-C9BE-443C-AD45-37F36434896B}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B4:G13">
-    <cfRule type="colorScale" priority="35">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -2457,28 +2705,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C18:C24">
-    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="blue">
+    <cfRule type="containsText" dxfId="12" priority="16" operator="containsText" text="blue">
       <formula>NOT(ISERROR(SEARCH("blue",C18)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C68:C79">
+    <cfRule type="dataBar" priority="2">
+      <dataBar showValue="0">
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color theme="5" tint="0.79998168889431442"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{5458FCFB-C965-4DCF-A2C7-3954E2FF0C3E}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D18:D24">
-    <cfRule type="timePeriod" dxfId="11" priority="8" timePeriod="tomorrow">
+    <cfRule type="timePeriod" dxfId="11" priority="13" timePeriod="tomorrow">
       <formula>FLOOR(D18,1)=TODAY()+1</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="10" priority="9" timePeriod="today">
+    <cfRule type="timePeriod" dxfId="10" priority="14" timePeriod="today">
       <formula>FLOOR(D18,1)=TODAY()</formula>
     </cfRule>
-    <cfRule type="timePeriod" dxfId="9" priority="10" timePeriod="yesterday">
+    <cfRule type="timePeriod" dxfId="9" priority="15" timePeriod="yesterday">
       <formula>FLOOR(D18,1)=TODAY()-1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D45:D51">
-    <cfRule type="expression" dxfId="8" priority="16">
+    <cfRule type="expression" dxfId="8" priority="21">
       <formula>D45 &gt; 2002</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D68:D79">
-    <cfRule type="dataBar" priority="34">
+    <cfRule type="dataBar" priority="39">
       <dataBar>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -2492,36 +2754,45 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E29:E37">
-    <cfRule type="aboveAverage" dxfId="7" priority="6" aboveAverage="0"/>
-    <cfRule type="aboveAverage" dxfId="6" priority="7"/>
+    <cfRule type="aboveAverage" dxfId="7" priority="11" aboveAverage="0"/>
+    <cfRule type="aboveAverage" dxfId="6" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45:E51">
-    <cfRule type="expression" dxfId="5" priority="31">
+    <cfRule type="expression" dxfId="5" priority="36">
       <formula>ISNUMBER(E45) = FALSE</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="33">
+    <cfRule type="expression" dxfId="4" priority="38">
       <formula>ISNUMBER(E45)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="G68:G79">
+    <cfRule type="iconSet" priority="4">
+      <iconSet>
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G18:I24">
-    <cfRule type="containsBlanks" dxfId="3" priority="37">
+    <cfRule type="containsBlanks" dxfId="3" priority="42">
       <formula>LEN(TRIM(G18))=0</formula>
     </cfRule>
-    <cfRule type="notContainsBlanks" dxfId="2" priority="38">
+    <cfRule type="notContainsBlanks" dxfId="2" priority="43">
       <formula>LEN(TRIM(G18))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:L23">
-    <cfRule type="notContainsErrors" dxfId="1" priority="39">
+    <cfRule type="notContainsErrors" dxfId="1" priority="44">
       <formula>NOT(ISERROR(L18))</formula>
     </cfRule>
-    <cfRule type="containsErrors" dxfId="0" priority="41">
+    <cfRule type="containsErrors" dxfId="0" priority="46">
       <formula>ISERROR(L18)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="10">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -2531,10 +2802,38 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{24D561F3-C9BE-443C-AD45-37F36434896B}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="formula">
+                <xm:f>30-5</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="formula">
+                <xm:f>120-5</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>B68:B79</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{5458FCFB-C965-4DCF-A2C7-3954E2FF0C3E}">
+            <x14:dataBar minLength="0" maxLength="100" border="1" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:borderColor rgb="FFED9D9B"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C68:C79</xm:sqref>
+        </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8DADE4BE-191E-4A96-91F5-C800E0B77060}">
             <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
@@ -2548,6 +2847,56 @@
           </x14:cfRule>
           <xm:sqref>D68:D79</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="5" id="{462FA517-799F-46DC-A679-14ACE54492E7}">
+            <x14:iconSet iconSet="5Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>20</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>40</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>60</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="percent">
+                <xm:f>80</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Flags" iconId="0"/>
+              <x14:cfIcon iconSet="4Arrows" iconId="1"/>
+              <x14:cfIcon iconSet="3Triangles" iconId="1"/>
+              <x14:cfIcon iconSet="4Arrows" iconId="2"/>
+              <x14:cfIcon iconSet="3Flags" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>H68:H79</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="iconSet" priority="3" id="{DF1B2F4E-D88B-402C-BF1F-467A4E628D4D}">
+            <x14:iconSet iconSet="4Arrows" custom="1">
+              <x14:cfvo type="percent">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>2</xm:f>
+              </x14:cfvo>
+              <x14:cfIcon iconSet="3Arrows" iconId="0"/>
+              <x14:cfIcon iconSet="4ArrowsGray" iconId="2"/>
+              <x14:cfIcon iconSet="4Arrows" iconId="2"/>
+              <x14:cfIcon iconSet="3Arrows" iconId="2"/>
+            </x14:iconSet>
+          </x14:cfRule>
+          <xm:sqref>I68:I79</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>